<commit_message>
Removed last two rows in the specimen tab because they contained no data.
</commit_message>
<xml_diff>
--- a/IYS2022_NW_Data.xlsx
+++ b/IYS2022_NW_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20391"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\GitHub\2022-NW-Data-Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24C2270-28B2-419B-806B-4436BCD694EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015CC26A-98DE-4CEA-97C9-D51CEB580E57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,14 @@
     <definedName name="__xlnm._FilterDatabase" localSheetId="3">Catch_Info!$C$1:$K$166</definedName>
     <definedName name="__xlnm._FilterDatabase_1">Catch_Info!$C$1:$K$166</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sampling_Event_Info!$A$1:$X$67</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Specimen_Info!$A$1:$S$1218</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Specimen_Info!$A$1:$S$1216</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16221" uniqueCount="1783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16217" uniqueCount="1783">
   <si>
     <t>Table</t>
   </si>
@@ -6437,10 +6437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S1218"/>
+  <dimension ref="A1:S1216"/>
   <sheetViews>
-    <sheetView topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="A1196" workbookViewId="0">
+      <selection activeCell="D1222" sqref="D1222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -70219,55 +70219,9 @@
         <v>1769</v>
       </c>
     </row>
-    <row r="1217" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M1217" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N1217" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O1217" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P1217" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q1217" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="R1217" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="S1217" s="4" t="s">
-        <v>1769</v>
-      </c>
-    </row>
-    <row r="1218" spans="13:19" x14ac:dyDescent="0.25">
-      <c r="M1218" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="N1218" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="O1218" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="P1218" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Q1218" s="4" t="s">
-        <v>1771</v>
-      </c>
-      <c r="R1218" s="4" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="S1218" s="4" t="s">
-        <v>1769</v>
-      </c>
-    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:S1218" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:S1216" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Fork length, Mantle length, Bell diameter, Standard length, Total length"</formula1>
@@ -70286,7 +70240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>